<commit_message>
Addition of flag to change CHN to HUB if desired.
</commit_message>
<xml_diff>
--- a/InputData/pop.xlsx
+++ b/InputData/pop.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Documents/COVID-19_ML/InputData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepharehart/RProjects/COVID-19_ML/InputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909FFBCF-9676-4E47-A9BA-493A807AB143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9845E24E-8A0A-D544-AC21-30FFE82D152A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{92BD616F-8AC9-034D-955E-CE3B9FE1CCDF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="398">
   <si>
     <t>PopTotal</t>
   </si>
@@ -1221,6 +1221,12 @@
   </si>
   <si>
     <t>PopTotal_1000s</t>
+  </si>
+  <si>
+    <t>Hubei</t>
+  </si>
+  <si>
+    <t>HUB</t>
   </si>
 </sst>
 </file>
@@ -1256,9 +1262,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1576,7 +1581,7 @@
   <dimension ref="A1:D199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+      <selection activeCell="F192" sqref="F192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4504,7 +4509,7 @@
         <v>97338.582999999999</v>
       </c>
       <c r="D195">
-        <f t="shared" ref="D195:D198" si="3">C195*1000</f>
+        <f t="shared" ref="D195:D199" si="3">C195*1000</f>
         <v>97338583</v>
       </c>
     </row>
@@ -4554,8 +4559,19 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C199" s="1"/>
-      <c r="D199" s="1"/>
+      <c r="A199" t="s">
+        <v>396</v>
+      </c>
+      <c r="B199" t="s">
+        <v>397</v>
+      </c>
+      <c r="C199">
+        <v>58500</v>
+      </c>
+      <c r="D199">
+        <f t="shared" si="3"/>
+        <v>58500000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>